<commit_message>
Add multi table test suite
</commit_message>
<xml_diff>
--- a/sample/excel/Simple_Template_With_Vertical_Int_Sort.xlsx
+++ b/sample/excel/Simple_Template_With_Vertical_Int_Sort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\rendr\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24621518-A9E2-41A7-A9E0-2C26FE103A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C4B11-2EF0-4DCC-9059-669B89A944B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="1065" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holdings" sheetId="1" r:id="rId1"/>
@@ -732,17 +732,17 @@
     <xf numFmtId="39" fontId="2" fillId="3" borderId="3" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="4" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="5" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="6" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="4" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="5" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="6" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:X155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -3642,13 +3642,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="67" t="s">
@@ -3699,125 +3699,132 @@
       <c r="A7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
@@ -3828,13 +3835,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>